<commit_message>
Updated with Selenium&Native Drag&Drop to bypass bug in selenium.
</commit_message>
<xml_diff>
--- a/WebDragNDrop/Main.rvl.xlsx
+++ b/WebDragNDrop/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="28">
   <si>
     <t>Flow</t>
   </si>
@@ -117,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="163">
+  <borders count="166">
     <border>
       <left/>
       <right/>
@@ -287,11 +287,14 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -455,6 +458,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="160" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="161" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="162" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="163" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="164" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="165" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,7 +470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H20"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.453125" customWidth="true"/>
@@ -604,7 +610,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
@@ -618,134 +624,114 @@
       <c r="H9" s="56"/>
     </row>
     <row r="10">
-      <c r="A10" s="57"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="64"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="80"/>
     </row>
     <row r="11">
-      <c r="A11" s="65"/>
-      <c r="B11" s="66"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="72"/>
+      <c r="A11" s="81"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="88"/>
     </row>
     <row r="12">
-      <c r="A12" s="73"/>
-      <c r="B12" s="74"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="80"/>
+      <c r="A12" s="89"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="95"/>
+      <c r="H12" s="96"/>
     </row>
     <row r="13">
-      <c r="A13" s="81"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="88"/>
+      <c r="A13" s="97"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="101"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="104"/>
     </row>
     <row r="14">
-      <c r="A14" s="89"/>
-      <c r="B14" s="90"/>
-      <c r="C14" s="91"/>
-      <c r="D14" s="92"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="95"/>
-      <c r="H14" s="96"/>
+      <c r="A14" s="105"/>
+      <c r="B14" s="106"/>
+      <c r="C14" s="107"/>
+      <c r="D14" s="108"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="110"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="112"/>
     </row>
     <row r="15">
-      <c r="A15" s="97"/>
-      <c r="B15" s="98"/>
-      <c r="C15" s="99"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="102"/>
-      <c r="G15" s="103"/>
-      <c r="H15" s="104"/>
+      <c r="A15" s="113"/>
+      <c r="B15" s="114"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="117"/>
+      <c r="F15" s="118"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="120"/>
     </row>
     <row r="16">
-      <c r="A16" s="105"/>
-      <c r="B16" s="106"/>
-      <c r="C16" s="107"/>
-      <c r="D16" s="108"/>
-      <c r="E16" s="109"/>
-      <c r="F16" s="110"/>
-      <c r="G16" s="111"/>
-      <c r="H16" s="112"/>
+      <c r="A16" s="121"/>
+      <c r="B16" s="122"/>
+      <c r="C16" s="123"/>
+      <c r="D16" s="124"/>
+      <c r="E16" s="125"/>
+      <c r="F16" s="126"/>
+      <c r="G16" s="127"/>
+      <c r="H16" s="128"/>
     </row>
     <row r="17">
-      <c r="A17" s="113"/>
-      <c r="B17" s="114"/>
-      <c r="C17" s="115"/>
-      <c r="D17" s="116"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="118"/>
-      <c r="G17" s="119"/>
-      <c r="H17" s="120"/>
+      <c r="A17" s="129"/>
+      <c r="B17" s="130"/>
+      <c r="C17" s="131"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="134"/>
+      <c r="G17" s="135"/>
+      <c r="H17" s="136"/>
     </row>
     <row r="18">
-      <c r="A18" s="121"/>
-      <c r="B18" s="122"/>
-      <c r="C18" s="123"/>
-      <c r="D18" s="124"/>
-      <c r="E18" s="125"/>
-      <c r="F18" s="126"/>
-      <c r="G18" s="127"/>
-      <c r="H18" s="128"/>
+      <c r="A18" s="137"/>
+      <c r="B18" s="138"/>
+      <c r="C18" s="139"/>
+      <c r="D18" s="140"/>
+      <c r="E18" s="141"/>
+      <c r="F18" s="142"/>
+      <c r="G18" s="143"/>
+      <c r="H18" s="144"/>
     </row>
     <row r="19">
-      <c r="A19" s="129"/>
-      <c r="B19" s="130"/>
-      <c r="C19" s="131"/>
-      <c r="D19" s="132"/>
-      <c r="E19" s="133"/>
-      <c r="F19" s="134"/>
-      <c r="G19" s="135"/>
-      <c r="H19" s="136"/>
+      <c r="A19" s="145"/>
+      <c r="B19" s="146"/>
+      <c r="C19" s="147"/>
+      <c r="D19" s="148"/>
+      <c r="E19" s="149"/>
+      <c r="F19" s="150"/>
+      <c r="G19" s="151"/>
+      <c r="H19" s="152"/>
     </row>
     <row r="20">
-      <c r="A20" s="137"/>
-      <c r="B20" s="138"/>
-      <c r="C20" s="139"/>
-      <c r="D20" s="140"/>
-      <c r="E20" s="141"/>
-      <c r="F20" s="142"/>
-      <c r="G20" s="143"/>
-      <c r="H20" s="144"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="145"/>
-      <c r="B21" s="146"/>
-      <c r="C21" s="147"/>
-      <c r="D21" s="148"/>
-      <c r="E21" s="149"/>
-      <c r="F21" s="150"/>
-      <c r="G21" s="151"/>
-      <c r="H21" s="152"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="153"/>
-      <c r="B22" s="154"/>
-      <c r="C22" s="155"/>
-      <c r="D22" s="156"/>
-      <c r="E22" s="157"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="159"/>
-      <c r="H22" s="160"/>
+      <c r="A20" s="153"/>
+      <c r="B20" s="154"/>
+      <c r="C20" s="155"/>
+      <c r="D20" s="156"/>
+      <c r="E20" s="157"/>
+      <c r="F20" s="158"/>
+      <c r="G20" s="159"/>
+      <c r="H20" s="160"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>